<commit_message>
Adding reader wavelength concentration units
</commit_message>
<xml_diff>
--- a/DnaRepairSpreadsheetParser/test/exampleData/minAssayAnnotationSpreadsheets/Broad Institute_MH.xlsx
+++ b/DnaRepairSpreadsheetParser/test/exampleData/minAssayAnnotationSpreadsheets/Broad Institute_MH.xlsx
@@ -382,12 +382,6 @@
     <t>GI:109633019</t>
   </si>
   <si>
-    <t>610nM</t>
-  </si>
-  <si>
-    <t>310nM</t>
-  </si>
-  <si>
     <t>GI:7468</t>
   </si>
   <si>
@@ -425,6 +419,12 @@
   </si>
   <si>
     <t>assay component role</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reader WaveLength </t>
+  </si>
+  <si>
+    <t>nanometer</t>
   </si>
 </sst>
 </file>
@@ -816,10 +816,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:BH9"/>
+  <dimension ref="A1:BI9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="V1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="W3" sqref="W3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -839,7 +839,7 @@
     <col min="55" max="58" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:60" s="2" customFormat="1" ht="156.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:61" s="2" customFormat="1" ht="156.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -948,8 +948,11 @@
       <c r="BF1" s="12"/>
       <c r="BG1" s="12"/>
       <c r="BH1" s="12"/>
+      <c r="BI1" s="2" t="s">
+        <v>127</v>
+      </c>
     </row>
-    <row r="2" spans="1:60" s="3" customFormat="1" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:61" s="3" customFormat="1" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>20</v>
       </c>
@@ -969,7 +972,7 @@
         <v>24</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>25</v>
@@ -1127,8 +1130,11 @@
       <c r="BG2" t="s">
         <v>108</v>
       </c>
+      <c r="BI2" s="3" t="s">
+        <v>128</v>
+      </c>
     </row>
-    <row r="3" spans="1:60" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:61" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>78</v>
       </c>
@@ -1140,7 +1146,7 @@
         <v>89</v>
       </c>
       <c r="D3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E3" t="s">
         <v>79</v>
@@ -1158,13 +1164,13 @@
         <v>113</v>
       </c>
       <c r="L3" s="9" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="M3" t="s">
         <v>93</v>
       </c>
       <c r="N3" s="9" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="O3" t="s">
         <v>83</v>
@@ -1187,17 +1193,17 @@
       <c r="U3" t="s">
         <v>92</v>
       </c>
-      <c r="V3" t="s">
-        <v>115</v>
-      </c>
-      <c r="W3" t="s">
-        <v>114</v>
+      <c r="V3">
+        <v>310</v>
+      </c>
+      <c r="W3">
+        <v>610</v>
       </c>
       <c r="Y3" t="s">
         <v>100</v>
       </c>
       <c r="Z3" s="9" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="AA3">
         <v>50</v>
@@ -1206,7 +1212,7 @@
         <v>91</v>
       </c>
       <c r="AC3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="AE3" t="s">
         <v>81</v>
@@ -1225,7 +1231,7 @@
       </c>
       <c r="AJ3" s="8"/>
       <c r="AK3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="AL3" t="s">
         <v>70</v>
@@ -1255,10 +1261,10 @@
         <v>77</v>
       </c>
       <c r="AV3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="AW3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="BA3" t="s">
         <v>1</v>
@@ -1282,7 +1288,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="4" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1293,7 +1299,7 @@
         <v>99</v>
       </c>
       <c r="I4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="J4">
         <v>5</v>
@@ -1302,13 +1308,13 @@
         <v>85</v>
       </c>
       <c r="L4" s="9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="M4" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="5" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -1319,28 +1325,28 @@
         <v>98</v>
       </c>
       <c r="L5" s="9" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="M5" s="10" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
-    <row r="6" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>1</v>
       </c>

</xml_diff>